<commit_message>
Text mit Editor, Versuch 3
</commit_message>
<xml_diff>
--- a/Excel_Test.xlsx
+++ b/Excel_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z003n6ue\Documents\Git\Test2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099D8C9E-189B-4F3F-8067-AE607CDC2A9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE61EB1-02B2-4B55-BBCC-E8937C1EC80D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="49170" yWindow="-9660" windowWidth="29040" windowHeight="17640" xr2:uid="{1EC71E23-2E67-4BE9-B195-861E56B9FD99}"/>
   </bookViews>
@@ -31,22 +31,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Version 1</t>
   </si>
   <si>
     <t>Version 2</t>
   </si>
+  <si>
+    <t>Version 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15A5549-D922-4126-9FF4-726C11275F4B}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +415,13 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>